<commit_message>
Solution to getting Excel Data
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sebastian 1/PycharmProjects/Campus-San_Valentin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sebastian 1/PycharmProjects/Campus_San_Val_Repo1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C648F93A-D698-EC41-B6EF-C1E55014CC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC621D-1F95-4A43-9BE5-8DF473813AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{11BB83DB-CBCA-0642-8990-382507911075}"/>
+    <workbookView xWindow="5480" yWindow="3340" windowWidth="35840" windowHeight="20120" xr2:uid="{11BB83DB-CBCA-0642-8990-382507911075}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E46333F-3F55-2E49-BE7A-6ABE0C1B23A0}">
-  <dimension ref="B2:E3"/>
+  <dimension ref="B2:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -416,7 +416,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -429,8 +429,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>4</v>
       </c>

</xml_diff>